<commit_message>
feat: update RICS background data
</commit_message>
<xml_diff>
--- a/references/background_data/RICS_service_life.xlsx
+++ b/references/background_data/RICS_service_life.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{86FAF29C-DF96-4A07-A3C6-D2DF30C60BE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B93176-EBF5-4014-A116-51E225117228}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RICS_service_life" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t xml:space="preserve">id	</t>
   </si>
@@ -116,12 +116,15 @@
   </si>
   <si>
     <t>service_lives</t>
+  </si>
+  <si>
+    <t>Assembly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -963,11 +966,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D46"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,8 +982,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
+      <c r="B1" t="s">
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -994,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1008,10 +1011,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>60</v>
@@ -1022,10 +1025,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -1036,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1050,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1064,7 +1067,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -1078,7 +1081,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1092,13 +1095,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1106,7 +1109,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1120,13 +1123,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1134,7 +1137,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1148,13 +1151,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1162,13 +1165,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D14">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,13 +1179,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1190,7 +1193,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1204,7 +1207,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1218,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -1232,13 +1235,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1246,7 +1249,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1259,13 +1262,27 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: create replacement prebuilt scenarios
</commit_message>
<xml_diff>
--- a/references/background_data/RICS_service_life.xlsx
+++ b/references/background_data/RICS_service_life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B93176-EBF5-4014-A116-51E225117228}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AAC2BC-9D4A-4D1C-8F38-0694BA0FE92E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
-    <t xml:space="preserve">id	</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>Assembly</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,16 +980,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -997,10 +997,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>60</v>
@@ -1011,10 +1011,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>60</v>
@@ -1025,10 +1025,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -1039,10 +1039,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>60</v>
@@ -1053,10 +1053,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -1067,10 +1067,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>60</v>
@@ -1081,10 +1081,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>60</v>
@@ -1095,10 +1095,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>60</v>
@@ -1109,10 +1109,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>35</v>
@@ -1123,10 +1123,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>35</v>
@@ -1137,10 +1137,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -1151,10 +1151,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>60</v>
@@ -1165,10 +1165,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>30</v>
@@ -1179,10 +1179,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>35</v>
@@ -1193,10 +1193,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>30</v>
@@ -1207,10 +1207,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>30</v>
@@ -1221,10 +1221,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>30</v>
@@ -1235,10 +1235,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>30</v>
@@ -1249,10 +1249,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <v>35</v>
@@ -1263,10 +1263,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>35</v>
@@ -1277,10 +1277,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>30</v>

</xml_diff>

<commit_message>
feat: more updates in background datasets
</commit_message>
<xml_diff>
--- a/references/background_data/RICS_service_life.xlsx
+++ b/references/background_data/RICS_service_life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AAC2BC-9D4A-4D1C-8F38-0694BA0FE92E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8009EF-6BE9-44B7-BD92-F4826B5E39BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>Curtain wall: steel spandrel</t>
   </si>
   <si>
-    <t>Curtain wall: alu spandrel</t>
-  </si>
-  <si>
     <t>MV: brick</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Curtain wall: aluminum spandrel</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,16 +980,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,7 +1123,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1137,7 +1137,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1151,7 +1151,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1165,7 +1165,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -1179,7 +1179,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1193,7 +1193,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1207,7 +1207,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -1221,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1235,7 +1235,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -1249,7 +1249,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -1263,7 +1263,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -1277,7 +1277,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
feat: add single family home data
</commit_message>
<xml_diff>
--- a/references/background_data/RICS_service_life.xlsx
+++ b/references/background_data/RICS_service_life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8009EF-6BE9-44B7-BD92-F4826B5E39BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F01D339-7579-432B-B369-6B14209F2482}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>type</t>
   </si>
@@ -119,6 +119,30 @@
   </si>
   <si>
     <t>Curtain wall: aluminum spandrel</t>
+  </si>
+  <si>
+    <t>Concrete footing</t>
+  </si>
+  <si>
+    <t>Floor framing</t>
+  </si>
+  <si>
+    <t>Sub-flooring</t>
+  </si>
+  <si>
+    <t>Roof framing</t>
+  </si>
+  <si>
+    <t>Roof decking</t>
+  </si>
+  <si>
+    <t>Brick: wood framing</t>
+  </si>
+  <si>
+    <t>Glazing: operable window</t>
+  </si>
+  <si>
+    <t>Asphalt shingle roofing</t>
   </si>
 </sst>
 </file>
@@ -967,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,8 +1034,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+      <c r="B3" t="s">
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1025,10 +1049,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -1039,10 +1063,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>60</v>
@@ -1053,7 +1077,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -1067,7 +1091,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -1081,7 +1105,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -1095,7 +1119,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -1109,13 +1133,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,13 +1147,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,10 +1161,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -1151,10 +1175,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>60</v>
@@ -1165,13 +1189,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,7 +1203,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1193,13 +1217,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D16">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1207,13 +1231,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,27 +1245,27 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
+      <c r="B19" t="s">
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1249,13 +1273,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D20">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1263,7 +1287,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -1276,13 +1300,125 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
         <v>7</v>
       </c>
-      <c r="D22">
+      <c r="D29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
         <v>30</v>
       </c>
     </row>

</xml_diff>